<commit_message>
Adjusted planing for sprint 2
</commit_message>
<xml_diff>
--- a/doc/task06/scrum_team_blue.xlsx
+++ b/doc/task06/scrum_team_blue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BFH\2019_Frühlingssemester\Software Engineering und Design\ch.bfh.bti7081.s2019.blue\doc\task06\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\studium\sem-4\BTI7081-SW-Engineering\_project\ch.bfh.bti7081.s2019.blue\doc\task06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C660E4F-04A1-4BC2-A723-2908FDC085B6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155B1EAC-F7D5-499F-9AC6-10AFA619FF26}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="81">
   <si>
     <t>ID</t>
   </si>
@@ -165,9 +165,6 @@
     <t>Den Rapport eines Einsatzes eines Spitex Mitarbeiters kontrollieren und freigeben</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Das planen der Patienteneinsätze</t>
   </si>
   <si>
@@ -226,6 +223,57 @@
   </si>
   <si>
     <t>Vorschlagsalgorithmus implementieren</t>
+  </si>
+  <si>
+    <t>MA kann einem Einsatz zugewiesen werden</t>
+  </si>
+  <si>
+    <t>Frontend für MA Zuweisung</t>
+  </si>
+  <si>
+    <t>Backend für MA Zuweisung</t>
+  </si>
+  <si>
+    <t>Backend für MA Zuweisungsvorschläge</t>
+  </si>
+  <si>
+    <t>Neue Mission Instanzen müssen erstellt werden, sobald einem Termin ein MA zugewiesen wird.</t>
+  </si>
+  <si>
+    <t>Frontend für Tagesübersicht MA erstellen</t>
+  </si>
+  <si>
+    <t>Backend für Tagesübersicht eines MA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Daten die auf der View dargestellt werden, müssen </t>
+  </si>
+  <si>
+    <t>HealthVisitor</t>
+  </si>
+  <si>
+    <t>Frontend für Terminvorschläge MA</t>
+  </si>
+  <si>
+    <t>Vorschläge nach Priorität sollen vorhanden sein, Terminkonflikte sollen berücksichtigt sein. Die Priorität ist nach Anzahl bisheriger Besuche festgelegt.</t>
+  </si>
+  <si>
+    <t>Backend für Terminvorschläge MA</t>
+  </si>
+  <si>
+    <t>Frontend für Terminvorschläge annehmen</t>
+  </si>
+  <si>
+    <t>Die Vorschläge sollen akzeptiert werden können. Die Akzeptierung des Vorschlags generiert eine neue Mission (Wie in 3.3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auf der MA Übersicht sollen für noch freie Termin Vorschläge gemacht werden. </t>
+  </si>
+  <si>
+    <t>Die Vorschläge sollen auf Anzahl bisheriger Besuche und freiem Terminkalender basieren</t>
+  </si>
+  <si>
+    <t>Alle Termine des aktuellen Tages sollen dargestellt werden. (Timeline)</t>
   </si>
 </sst>
 </file>
@@ -281,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -299,6 +347,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -639,7 +690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -704,10 +755,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -782,7 +833,7 @@
         <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -831,16 +882,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="s">
         <v>63</v>
-      </c>
-      <c r="C5" t="s">
-        <v>64</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
       </c>
       <c r="E5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -857,16 +908,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E6">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -883,16 +934,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -928,23 +979,6 @@
       </c>
       <c r="H8" s="1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="D10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10">
-        <f>SUM(E2:E8)</f>
-        <v>150</v>
-      </c>
-      <c r="F10">
-        <f>SUM(F2:F8)</f>
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <f>SUM(G2:G8)</f>
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -955,18 +989,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="4.7890625" customWidth="1"/>
     <col min="2" max="2" width="6.20703125" customWidth="1"/>
-    <col min="3" max="3" width="25.3125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.05078125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.89453125" customWidth="1"/>
     <col min="6" max="6" width="9.20703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.7890625" customWidth="1"/>
@@ -1023,19 +1057,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
         <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H2" t="s">
         <v>5</v>
@@ -1061,19 +1095,19 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D3" t="s">
-        <v>48</v>
-      </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" t="s">
         <v>56</v>
-      </c>
-      <c r="G3" t="s">
-        <v>57</v>
       </c>
       <c r="H3" t="s">
         <v>5</v>
@@ -1099,19 +1133,19 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>61</v>
       </c>
-      <c r="E4" t="s">
-        <v>62</v>
-      </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H4" t="s">
         <v>5</v>
@@ -1137,19 +1171,19 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" t="s">
-        <v>52</v>
+        <v>49</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H5" t="s">
         <v>6</v>
@@ -1175,19 +1209,19 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
         <v>53</v>
       </c>
-      <c r="E6" t="s">
-        <v>54</v>
-      </c>
       <c r="F6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H6" t="s">
         <v>6</v>
@@ -1202,6 +1236,310 @@
         <v>0</v>
       </c>
       <c r="L6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>3.1</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>3.2</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="25.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>3.3</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11">
+        <v>5</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>4.2</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12">
+        <v>10</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>4.3</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13">
+        <v>5</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14">
+        <v>10</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>5.2</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15">
+        <v>5</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1215,7 +1553,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Adjusted planing for sprint 2 (#38)
* Adjusted planing for sprint 2

* Finished sprint planing
</commit_message>
<xml_diff>
--- a/doc/task06/scrum_team_blue.xlsx
+++ b/doc/task06/scrum_team_blue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BFH\2019_Frühlingssemester\Software Engineering und Design\ch.bfh.bti7081.s2019.blue\doc\task06\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\studium\sem-4\BTI7081-SW-Engineering\_project\ch.bfh.bti7081.s2019.blue\doc\task06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C660E4F-04A1-4BC2-A723-2908FDC085B6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DA7D2F-2882-426D-9DDD-CA976EC3DB8C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="82">
   <si>
     <t>ID</t>
   </si>
@@ -165,21 +165,9 @@
     <t>Den Rapport eines Einsatzes eines Spitex Mitarbeiters kontrollieren und freigeben</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Das planen der Patienteneinsätze</t>
   </si>
   <si>
-    <t>Domain Model erstellen</t>
-  </si>
-  <si>
-    <t>Wochenplanung GUI</t>
-  </si>
-  <si>
-    <t>View und Presenter</t>
-  </si>
-  <si>
     <t>Klassen Patient, Adresse, Mission, Health Visitor und Task erstellen</t>
   </si>
   <si>
@@ -189,12 +177,6 @@
     <t>Logik der Patienteneinsätze</t>
   </si>
   <si>
-    <t>Frontend</t>
-  </si>
-  <si>
-    <t>Backend</t>
-  </si>
-  <si>
     <t>Planung</t>
   </si>
   <si>
@@ -216,9 +198,6 @@
     <t>Basis für Layering Pattern legen</t>
   </si>
   <si>
-    <t>Business-, Persistenzservice und API</t>
-  </si>
-  <si>
     <t>Layering</t>
   </si>
   <si>
@@ -226,6 +205,78 @@
   </si>
   <si>
     <t>Vorschlagsalgorithmus implementieren</t>
+  </si>
+  <si>
+    <t>MA kann einem Einsatz zugewiesen werden</t>
+  </si>
+  <si>
+    <t>Frontend für MA Zuweisung</t>
+  </si>
+  <si>
+    <t>Backend für MA Zuweisung</t>
+  </si>
+  <si>
+    <t>Backend für MA Zuweisungsvorschläge</t>
+  </si>
+  <si>
+    <t>Neue Mission Instanzen müssen erstellt werden, sobald einem Termin ein MA zugewiesen wird.</t>
+  </si>
+  <si>
+    <t>Frontend für Tagesübersicht MA erstellen</t>
+  </si>
+  <si>
+    <t>Backend für Tagesübersicht eines MA</t>
+  </si>
+  <si>
+    <t>HealthVisitor</t>
+  </si>
+  <si>
+    <t>Frontend für Terminvorschläge MA</t>
+  </si>
+  <si>
+    <t>Vorschläge nach Priorität sollen vorhanden sein, Terminkonflikte sollen berücksichtigt sein. Die Priorität ist nach Anzahl bisheriger Besuche festgelegt.</t>
+  </si>
+  <si>
+    <t>Backend für Terminvorschläge MA</t>
+  </si>
+  <si>
+    <t>Frontend für Terminvorschläge annehmen</t>
+  </si>
+  <si>
+    <t>Die Vorschläge sollen akzeptiert werden können. Die Akzeptierung des Vorschlags generiert eine neue Mission (Wie in 3.3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auf der MA Übersicht sollen für noch freie Termin Vorschläge gemacht werden. </t>
+  </si>
+  <si>
+    <t>Die Vorschläge sollen auf Anzahl bisheriger Besuche und freiem Terminkalender basieren</t>
+  </si>
+  <si>
+    <t>Domain Model &amp; Testdaten erstellen</t>
+  </si>
+  <si>
+    <t>Business-, Persistenzservice und API sollen vorhanden sein</t>
+  </si>
+  <si>
+    <t>Die View für das Erfassen von neuen Patienten Einsätzen muss vorhanden sein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend Logik für das Erfassen von neuen Einsätzen muss vorhanden sein. Terminkonflikte müssen verhindert werden. </t>
+  </si>
+  <si>
+    <t>Wochenplanung für MA &amp; Patient</t>
+  </si>
+  <si>
+    <t>Frontend und Backend für die MA-View und die Patienten-View muss erstellt werden. Es soll ein Kalender dargestellt werden, welcher Termine einer Woche beinhaltet.</t>
+  </si>
+  <si>
+    <t>Die Daten die auf der View dargestellt werden, müssen geliefert werden.</t>
+  </si>
+  <si>
+    <t>Alle Termine des aktuellen Tages sollen dargestellt werden. (Timeline)               Einsatz starten &amp; Einsatz beenden sollen vorhanden sein (nicht funktionstüchtig)</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -281,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -299,6 +350,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -639,7 +693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -704,10 +758,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -782,7 +836,7 @@
         <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -831,16 +885,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
       </c>
       <c r="E5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -857,16 +911,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E6">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -883,16 +937,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -928,23 +982,6 @@
       </c>
       <c r="H8" s="1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="D10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10">
-        <f>SUM(E2:E8)</f>
-        <v>150</v>
-      </c>
-      <c r="F10">
-        <f>SUM(F2:F8)</f>
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <f>SUM(G2:G8)</f>
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -955,18 +992,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="4.7890625" customWidth="1"/>
     <col min="2" max="2" width="6.20703125" customWidth="1"/>
-    <col min="3" max="3" width="25.3125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.05078125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.89453125" customWidth="1"/>
     <col min="6" max="6" width="9.20703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.7890625" customWidth="1"/>
@@ -1023,19 +1060,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
         <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="H2" t="s">
         <v>5</v>
@@ -1043,17 +1080,14 @@
       <c r="I2">
         <v>10</v>
       </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
       <c r="K2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="L2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="57.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>1.2</v>
       </c>
@@ -1061,19 +1095,19 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" t="s">
         <v>48</v>
       </c>
-      <c r="E3" t="s">
-        <v>54</v>
-      </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="G3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H3" t="s">
         <v>5</v>
@@ -1081,17 +1115,14 @@
       <c r="I3">
         <v>10</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
       <c r="K3">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="L3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>1.3</v>
       </c>
@@ -1099,19 +1130,19 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" t="s">
-        <v>61</v>
+        <v>54</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="G4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H4" t="s">
         <v>5</v>
@@ -1119,17 +1150,14 @@
       <c r="I4">
         <v>10</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
       <c r="K4">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="L4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>2.1</v>
       </c>
@@ -1137,19 +1165,19 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" t="s">
         <v>52</v>
-      </c>
-      <c r="E5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" t="s">
-        <v>58</v>
-      </c>
-      <c r="G5" t="s">
-        <v>56</v>
       </c>
       <c r="H5" t="s">
         <v>6</v>
@@ -1157,17 +1185,14 @@
       <c r="I5">
         <v>10</v>
       </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
       <c r="K5">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="L5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>2.2000000000000002</v>
       </c>
@@ -1175,19 +1200,19 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" t="s">
         <v>51</v>
-      </c>
-      <c r="D6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" t="s">
-        <v>59</v>
-      </c>
-      <c r="G6" t="s">
-        <v>58</v>
       </c>
       <c r="H6" t="s">
         <v>6</v>
@@ -1195,13 +1220,290 @@
       <c r="I6">
         <v>5</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
       <c r="K6">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="L6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>3.1</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>3.2</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>3.3</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11">
+        <v>5</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>4.2</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12">
+        <v>10</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>4.3</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13">
+        <v>5</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14">
+        <v>10</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>5.2</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15">
+        <v>5</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1215,7 +1517,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Updated product backlog with new story (overall-calendar)
</commit_message>
<xml_diff>
--- a/doc/task06/scrum_team_blue.xlsx
+++ b/doc/task06/scrum_team_blue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\studium\sem-4\BTI7081-SW-Engineering\_project\ch.bfh.bti7081.s2019.blue\doc\task06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DA7D2F-2882-426D-9DDD-CA976EC3DB8C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9107B16C-9A15-4211-A0C8-9B56E8A9691E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="84">
   <si>
     <t>ID</t>
   </si>
@@ -277,6 +277,12 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>Ressourcen Übersicht</t>
+  </si>
+  <si>
+    <t>Auf einem Kalender sollen alle MA Einsätze dargestellt werden</t>
   </si>
 </sst>
 </file>
@@ -758,10 +764,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -984,6 +990,32 @@
         <v>8</v>
       </c>
     </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>25</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -994,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Updated product backlog with new story (overall-calendar) (#51)
</commit_message>
<xml_diff>
--- a/doc/task06/scrum_team_blue.xlsx
+++ b/doc/task06/scrum_team_blue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\studium\sem-4\BTI7081-SW-Engineering\_project\ch.bfh.bti7081.s2019.blue\doc\task06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DA7D2F-2882-426D-9DDD-CA976EC3DB8C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9107B16C-9A15-4211-A0C8-9B56E8A9691E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="84">
   <si>
     <t>ID</t>
   </si>
@@ -277,6 +277,12 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>Ressourcen Übersicht</t>
+  </si>
+  <si>
+    <t>Auf einem Kalender sollen alle MA Einsätze dargestellt werden</t>
   </si>
 </sst>
 </file>
@@ -758,10 +764,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -984,6 +990,32 @@
         <v>8</v>
       </c>
     </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>25</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -994,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>